<commit_message>
textbox and table styling moved to styles.css
</commit_message>
<xml_diff>
--- a/content/blog/DH/calculations.xlsx
+++ b/content/blog/DH/calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\takat\OneDrive\Documents\Programming\Blog\eti-blog\content\blog\DH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4761A179-6492-48DA-9E0F-9BA8FB2B946F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566701C8-07A0-43DA-9A29-62133815BF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7B1EFD27-E7A9-4511-B124-4379698E9A90}"/>
   </bookViews>
@@ -1437,15 +1437,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1793,7 +1793,7 @@
   <dimension ref="A2:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>